<commit_message>
Mise à jour du backend
</commit_message>
<xml_diff>
--- a/backend/uploads/Feuil2.xlsx
+++ b/backend/uploads/Feuil2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\YOL2-FIC-01\Utilisateurs$\and.vespuce\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28FDBC68-EBE9-436D-BAAD-4063CFE7344D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD17043-C758-403F-8E1F-95F1AA75FCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" xr2:uid="{283D1B77-55FE-45D0-8D91-BD52EDA226B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{283D1B77-55FE-45D0-8D91-BD52EDA226B8}"/>
   </bookViews>
   <sheets>
     <sheet name="L-M1 MAPI ALT 1 - ALT Semes-1" sheetId="1" r:id="rId1"/>
@@ -1002,14 +1002,14 @@
     <t>14,49</t>
   </si>
   <si>
-    <t>* Attention, le total des absences prend en compte toutes les absences aux séances sur la période concernée. S'il existe des absences sur des matières qui ne figurent pas dans le relevé, elles seront également comptabilisées.</t>
+    <t>Nom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,8 +1036,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1059,6 +1065,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1352,7 +1364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1360,12 +1372,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1384,18 +1391,46 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1409,9 +1444,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1449,7 +1484,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1555,7 +1590,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1697,7 +1732,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1705,9 +1740,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC92F3-8B03-4ADB-96A2-2DD03D8E04BE}">
-  <dimension ref="B1:BM36"/>
+  <dimension ref="B1:BM34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1783,452 +1820,455 @@
       </c>
     </row>
     <row r="3" spans="2:65" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="2:65" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9" t="s">
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9" t="s">
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="9" t="s">
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="9" t="s">
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="9" t="s">
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="9" t="s">
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="9" t="s">
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="9" t="s">
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="9" t="s">
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="9" t="s">
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="AK4" s="8"/>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="9" t="s">
+      <c r="AK4" s="35"/>
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="8"/>
-      <c r="AP4" s="9" t="s">
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="35"/>
+      <c r="AP4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="8"/>
-      <c r="AS4" s="9" t="s">
+      <c r="AQ4" s="35"/>
+      <c r="AR4" s="35"/>
+      <c r="AS4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="AT4" s="8"/>
-      <c r="AU4" s="8"/>
-      <c r="AV4" s="9" t="s">
+      <c r="AT4" s="35"/>
+      <c r="AU4" s="35"/>
+      <c r="AV4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="AW4" s="8"/>
-      <c r="AX4" s="8"/>
-      <c r="AY4" s="9" t="s">
+      <c r="AW4" s="35"/>
+      <c r="AX4" s="35"/>
+      <c r="AY4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="AZ4" s="8"/>
-      <c r="BA4" s="8"/>
-      <c r="BB4" s="9" t="s">
+      <c r="AZ4" s="35"/>
+      <c r="BA4" s="35"/>
+      <c r="BB4" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="BC4" s="8"/>
-      <c r="BD4" s="8"/>
-      <c r="BE4" s="9" t="s">
+      <c r="BC4" s="35"/>
+      <c r="BD4" s="35"/>
+      <c r="BE4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="BF4" s="8"/>
-      <c r="BG4" s="8"/>
-      <c r="BH4" s="9" t="s">
+      <c r="BF4" s="35"/>
+      <c r="BG4" s="35"/>
+      <c r="BH4" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="BI4" s="8"/>
-      <c r="BJ4" s="8"/>
-      <c r="BK4" s="31" t="s">
+      <c r="BI4" s="35"/>
+      <c r="BJ4" s="35"/>
+      <c r="BK4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="BL4" s="10"/>
-      <c r="BM4" s="12"/>
+      <c r="BL4" s="37"/>
+      <c r="BM4" s="38"/>
     </row>
     <row r="5" spans="2:65" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="B5" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="E5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="17" t="s">
+      <c r="H5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="17" t="s">
+      <c r="K5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="17" t="s">
+      <c r="N5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="S5" s="17" t="s">
+      <c r="Q5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="U5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="V5" s="17" t="s">
+      <c r="T5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="W5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="X5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y5" s="17" t="s">
+      <c r="W5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Z5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB5" s="17" t="s">
+      <c r="Z5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AC5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE5" s="17" t="s">
+      <c r="AC5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AF5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH5" s="17" t="s">
+      <c r="AF5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AI5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK5" s="17" t="s">
+      <c r="AI5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AL5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AM5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN5" s="17" t="s">
+      <c r="AL5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AO5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ5" s="17" t="s">
+      <c r="AO5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AR5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT5" s="17" t="s">
+      <c r="AR5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AU5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AV5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW5" s="17" t="s">
+      <c r="AU5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AX5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ5" s="17" t="s">
+      <c r="AX5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BA5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="BB5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC5" s="17" t="s">
+      <c r="BA5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BD5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BF5" s="17" t="s">
+      <c r="BD5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BG5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="BH5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="BI5" s="17" t="s">
+      <c r="BG5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BJ5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="BK5" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="BL5" s="11" t="s">
+      <c r="BJ5" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="BK5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="BM5" s="13" t="s">
+      <c r="BM5" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="20">
+      <c r="C6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="15">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="20">
-        <v>2</v>
-      </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="19" t="s">
+      <c r="G6" s="15">
+        <v>2</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="20">
-        <v>2</v>
-      </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="19" t="s">
+      <c r="J6" s="15">
+        <v>2</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="20">
-        <v>2</v>
-      </c>
-      <c r="N6" s="20"/>
-      <c r="O6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="P6" s="20">
+      <c r="M6" s="15">
+        <v>2</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="15">
         <v>3</v>
       </c>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="19" t="s">
+      <c r="Q6" s="15"/>
+      <c r="R6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="S6" s="20">
+      <c r="S6" s="15">
         <v>3</v>
       </c>
-      <c r="T6" s="20"/>
-      <c r="U6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="V6" s="20">
-        <v>4</v>
-      </c>
-      <c r="W6" s="20"/>
-      <c r="X6" s="19" t="s">
+      <c r="T6" s="15"/>
+      <c r="U6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="V6" s="15">
+        <v>4</v>
+      </c>
+      <c r="W6" s="15"/>
+      <c r="X6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="Y6" s="20">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="19" t="s">
+      <c r="Y6" s="15">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AB6" s="20">
-        <v>2</v>
-      </c>
-      <c r="AC6" s="20"/>
-      <c r="AD6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE6" s="20">
+      <c r="AB6" s="15">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE6" s="15">
         <v>11</v>
       </c>
-      <c r="AF6" s="20"/>
-      <c r="AG6" s="19" t="s">
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AH6" s="20">
-        <v>2</v>
-      </c>
-      <c r="AI6" s="20"/>
-      <c r="AJ6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK6" s="20"/>
-      <c r="AL6" s="20"/>
-      <c r="AM6" s="19" t="s">
+      <c r="AH6" s="15">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AN6" s="20"/>
-      <c r="AO6" s="20"/>
-      <c r="AP6" s="19" t="s">
+      <c r="AN6" s="15"/>
+      <c r="AO6" s="15"/>
+      <c r="AP6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AQ6" s="20"/>
-      <c r="AR6" s="20"/>
-      <c r="AS6" s="19" t="s">
+      <c r="AQ6" s="15"/>
+      <c r="AR6" s="15"/>
+      <c r="AS6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AT6" s="20">
+      <c r="AT6" s="15">
         <v>9</v>
       </c>
-      <c r="AU6" s="20"/>
-      <c r="AV6" s="19" t="s">
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AW6" s="20"/>
-      <c r="AX6" s="20"/>
-      <c r="AY6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="AZ6" s="20">
-        <v>4</v>
-      </c>
-      <c r="BA6" s="20"/>
-      <c r="BB6" s="19" t="s">
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="15"/>
+      <c r="AY6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ6" s="15">
+        <v>4</v>
+      </c>
+      <c r="BA6" s="15"/>
+      <c r="BB6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="BC6" s="20">
-        <v>2</v>
-      </c>
-      <c r="BD6" s="20"/>
-      <c r="BE6" s="19" t="s">
+      <c r="BC6" s="15">
+        <v>2</v>
+      </c>
+      <c r="BD6" s="15"/>
+      <c r="BE6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="BF6" s="20">
-        <v>2</v>
-      </c>
-      <c r="BG6" s="20"/>
-      <c r="BH6" s="19" t="s">
+      <c r="BF6" s="15">
+        <v>2</v>
+      </c>
+      <c r="BG6" s="15"/>
+      <c r="BH6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="BI6" s="20">
-        <v>2</v>
-      </c>
-      <c r="BJ6" s="27"/>
-      <c r="BK6" s="33" t="s">
+      <c r="BI6" s="15">
+        <v>2</v>
+      </c>
+      <c r="BJ6" s="22"/>
+      <c r="BK6" s="27" t="s">
         <v>41</v>
       </c>
       <c r="BL6" s="6">
         <v>28</v>
       </c>
-      <c r="BM6" s="37" t="s">
+      <c r="BM6" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2364,19 +2404,19 @@
       <c r="BI7" s="4">
         <v>2</v>
       </c>
-      <c r="BJ7" s="28"/>
-      <c r="BK7" s="34" t="s">
+      <c r="BJ7" s="23"/>
+      <c r="BK7" s="28" t="s">
         <v>58</v>
       </c>
       <c r="BL7" s="4">
         <v>26</v>
       </c>
-      <c r="BM7" s="23" t="s">
+      <c r="BM7" s="18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -2512,19 +2552,19 @@
       <c r="BI8" s="2">
         <v>2</v>
       </c>
-      <c r="BJ8" s="29"/>
-      <c r="BK8" s="35" t="s">
+      <c r="BJ8" s="24"/>
+      <c r="BK8" s="29" t="s">
         <v>69</v>
       </c>
       <c r="BL8" s="2">
         <v>28</v>
       </c>
-      <c r="BM8" s="24" t="s">
+      <c r="BM8" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2658,19 +2698,19 @@
       <c r="BI9" s="4">
         <v>2</v>
       </c>
-      <c r="BJ9" s="28"/>
-      <c r="BK9" s="34" t="s">
+      <c r="BJ9" s="23"/>
+      <c r="BK9" s="28" t="s">
         <v>80</v>
       </c>
       <c r="BL9" s="4">
         <v>28</v>
       </c>
-      <c r="BM9" s="23" t="s">
+      <c r="BM9" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>81</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -2806,19 +2846,19 @@
       <c r="BI10" s="2">
         <v>2</v>
       </c>
-      <c r="BJ10" s="29"/>
-      <c r="BK10" s="35" t="s">
+      <c r="BJ10" s="24"/>
+      <c r="BK10" s="29" t="s">
         <v>92</v>
       </c>
       <c r="BL10" s="2">
         <v>25</v>
       </c>
-      <c r="BM10" s="24" t="s">
+      <c r="BM10" s="19" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -2958,19 +2998,19 @@
       <c r="BI11" s="4">
         <v>2</v>
       </c>
-      <c r="BJ11" s="28"/>
-      <c r="BK11" s="34" t="s">
+      <c r="BJ11" s="23"/>
+      <c r="BK11" s="28" t="s">
         <v>102</v>
       </c>
       <c r="BL11" s="4">
         <v>25</v>
       </c>
-      <c r="BM11" s="23" t="s">
+      <c r="BM11" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="9" t="s">
         <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -3120,21 +3160,21 @@
       <c r="BI12" s="2">
         <v>2</v>
       </c>
-      <c r="BJ12" s="29" t="s">
+      <c r="BJ12" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="BK12" s="35" t="s">
+      <c r="BK12" s="29" t="s">
         <v>116</v>
       </c>
       <c r="BL12" s="2">
         <v>26</v>
       </c>
-      <c r="BM12" s="24" t="s">
+      <c r="BM12" s="19" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="10" t="s">
         <v>118</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -3270,19 +3310,19 @@
       <c r="BI13" s="4">
         <v>2</v>
       </c>
-      <c r="BJ13" s="28"/>
-      <c r="BK13" s="34" t="s">
+      <c r="BJ13" s="23"/>
+      <c r="BK13" s="28" t="s">
         <v>128</v>
       </c>
       <c r="BL13" s="4">
         <v>28</v>
       </c>
-      <c r="BM13" s="23" t="s">
+      <c r="BM13" s="18" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="14" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>129</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -3416,19 +3456,19 @@
       <c r="BI14" s="2">
         <v>2</v>
       </c>
-      <c r="BJ14" s="29"/>
-      <c r="BK14" s="35" t="s">
+      <c r="BJ14" s="24"/>
+      <c r="BK14" s="29" t="s">
         <v>136</v>
       </c>
       <c r="BL14" s="2">
         <v>25</v>
       </c>
-      <c r="BM14" s="24" t="s">
+      <c r="BM14" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>137</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -3566,19 +3606,19 @@
       <c r="BI15" s="4">
         <v>2</v>
       </c>
-      <c r="BJ15" s="28"/>
-      <c r="BK15" s="34" t="s">
+      <c r="BJ15" s="23"/>
+      <c r="BK15" s="28" t="s">
         <v>147</v>
       </c>
       <c r="BL15" s="4">
         <v>25</v>
       </c>
-      <c r="BM15" s="23" t="s">
+      <c r="BM15" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="16" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="9" t="s">
         <v>149</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -3716,19 +3756,19 @@
       <c r="BI16" s="2">
         <v>2</v>
       </c>
-      <c r="BJ16" s="29"/>
-      <c r="BK16" s="35" t="s">
+      <c r="BJ16" s="24"/>
+      <c r="BK16" s="29" t="s">
         <v>158</v>
       </c>
       <c r="BL16" s="2">
         <v>25</v>
       </c>
-      <c r="BM16" s="24" t="s">
+      <c r="BM16" s="19" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="10" t="s">
         <v>159</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -3862,19 +3902,19 @@
       <c r="BI17" s="4">
         <v>2</v>
       </c>
-      <c r="BJ17" s="28"/>
-      <c r="BK17" s="34" t="s">
+      <c r="BJ17" s="23"/>
+      <c r="BK17" s="28" t="s">
         <v>167</v>
       </c>
       <c r="BL17" s="4">
         <v>28</v>
       </c>
-      <c r="BM17" s="23" t="s">
+      <c r="BM17" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="9" t="s">
         <v>168</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -4014,21 +4054,21 @@
       <c r="BI18" s="2">
         <v>2</v>
       </c>
-      <c r="BJ18" s="29" t="s">
+      <c r="BJ18" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="BK18" s="35" t="s">
+      <c r="BK18" s="29" t="s">
         <v>178</v>
       </c>
       <c r="BL18" s="2">
         <v>28</v>
       </c>
-      <c r="BM18" s="24" t="s">
+      <c r="BM18" s="19" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="19" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="10" t="s">
         <v>180</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4162,19 +4202,19 @@
       <c r="BI19" s="4">
         <v>2</v>
       </c>
-      <c r="BJ19" s="28"/>
-      <c r="BK19" s="34" t="s">
+      <c r="BJ19" s="23"/>
+      <c r="BK19" s="28" t="s">
         <v>188</v>
       </c>
       <c r="BL19" s="4">
         <v>28</v>
       </c>
-      <c r="BM19" s="23" t="s">
+      <c r="BM19" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="9" t="s">
         <v>189</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -4308,19 +4348,19 @@
       <c r="BI20" s="2">
         <v>2</v>
       </c>
-      <c r="BJ20" s="29"/>
-      <c r="BK20" s="35" t="s">
+      <c r="BJ20" s="24"/>
+      <c r="BK20" s="29" t="s">
         <v>196</v>
       </c>
       <c r="BL20" s="2">
         <v>16</v>
       </c>
-      <c r="BM20" s="24" t="s">
+      <c r="BM20" s="19" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="10" t="s">
         <v>198</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -4456,19 +4496,19 @@
       <c r="BI21" s="4">
         <v>2</v>
       </c>
-      <c r="BJ21" s="28"/>
-      <c r="BK21" s="34" t="s">
+      <c r="BJ21" s="23"/>
+      <c r="BK21" s="28" t="s">
         <v>204</v>
       </c>
       <c r="BL21" s="4">
         <v>23</v>
       </c>
-      <c r="BM21" s="23" t="s">
+      <c r="BM21" s="18" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="9" t="s">
         <v>205</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -4602,19 +4642,19 @@
       <c r="BI22" s="2">
         <v>2</v>
       </c>
-      <c r="BJ22" s="29"/>
-      <c r="BK22" s="35" t="s">
+      <c r="BJ22" s="24"/>
+      <c r="BK22" s="29" t="s">
         <v>212</v>
       </c>
       <c r="BL22" s="2">
         <v>19</v>
       </c>
-      <c r="BM22" s="24" t="s">
+      <c r="BM22" s="19" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="10" t="s">
         <v>213</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -4750,19 +4790,19 @@
       <c r="BI23" s="4">
         <v>2</v>
       </c>
-      <c r="BJ23" s="28"/>
-      <c r="BK23" s="34" t="s">
+      <c r="BJ23" s="23"/>
+      <c r="BK23" s="28" t="s">
         <v>218</v>
       </c>
       <c r="BL23" s="4">
         <v>28</v>
       </c>
-      <c r="BM23" s="23" t="s">
+      <c r="BM23" s="18" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="24" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="9" t="s">
         <v>219</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -4900,19 +4940,19 @@
       <c r="BI24" s="2">
         <v>2</v>
       </c>
-      <c r="BJ24" s="29"/>
-      <c r="BK24" s="35" t="s">
+      <c r="BJ24" s="24"/>
+      <c r="BK24" s="29" t="s">
         <v>226</v>
       </c>
       <c r="BL24" s="2">
         <v>28</v>
       </c>
-      <c r="BM24" s="24" t="s">
+      <c r="BM24" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="25" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="10" t="s">
         <v>227</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -5046,19 +5086,19 @@
       <c r="BI25" s="4">
         <v>2</v>
       </c>
-      <c r="BJ25" s="28"/>
-      <c r="BK25" s="34" t="s">
+      <c r="BJ25" s="23"/>
+      <c r="BK25" s="28" t="s">
         <v>232</v>
       </c>
       <c r="BL25" s="4">
         <v>28</v>
       </c>
-      <c r="BM25" s="23" t="s">
+      <c r="BM25" s="18" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="9" t="s">
         <v>233</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -5192,19 +5232,19 @@
       <c r="BI26" s="2">
         <v>2</v>
       </c>
-      <c r="BJ26" s="29"/>
-      <c r="BK26" s="35" t="s">
+      <c r="BJ26" s="24"/>
+      <c r="BK26" s="29" t="s">
         <v>242</v>
       </c>
       <c r="BL26" s="2">
         <v>28</v>
       </c>
-      <c r="BM26" s="24" t="s">
+      <c r="BM26" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -5338,19 +5378,19 @@
       <c r="BI27" s="4">
         <v>2</v>
       </c>
-      <c r="BJ27" s="28"/>
-      <c r="BK27" s="34" t="s">
+      <c r="BJ27" s="23"/>
+      <c r="BK27" s="28" t="s">
         <v>250</v>
       </c>
       <c r="BL27" s="4">
         <v>28</v>
       </c>
-      <c r="BM27" s="23" t="s">
+      <c r="BM27" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="9" t="s">
         <v>251</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -5484,19 +5524,19 @@
       <c r="BI28" s="2">
         <v>2</v>
       </c>
-      <c r="BJ28" s="29"/>
-      <c r="BK28" s="35" t="s">
+      <c r="BJ28" s="24"/>
+      <c r="BK28" s="29" t="s">
         <v>257</v>
       </c>
       <c r="BL28" s="2">
         <v>28</v>
       </c>
-      <c r="BM28" s="24" t="s">
+      <c r="BM28" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="10" t="s">
         <v>258</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -5632,19 +5672,19 @@
       <c r="BI29" s="4">
         <v>2</v>
       </c>
-      <c r="BJ29" s="28"/>
-      <c r="BK29" s="34" t="s">
+      <c r="BJ29" s="23"/>
+      <c r="BK29" s="28" t="s">
         <v>266</v>
       </c>
       <c r="BL29" s="4">
         <v>25</v>
       </c>
-      <c r="BM29" s="23" t="s">
+      <c r="BM29" s="18" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="30" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="9" t="s">
         <v>267</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -5774,21 +5814,21 @@
         <v>279</v>
       </c>
       <c r="BI30" s="2"/>
-      <c r="BJ30" s="29" t="s">
+      <c r="BJ30" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="BK30" s="35" t="s">
+      <c r="BK30" s="29" t="s">
         <v>280</v>
       </c>
       <c r="BL30" s="2">
         <v>2</v>
       </c>
-      <c r="BM30" s="24" t="s">
+      <c r="BM30" s="19" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="31" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="10" t="s">
         <v>282</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -5924,19 +5964,19 @@
       <c r="BI31" s="4">
         <v>2</v>
       </c>
-      <c r="BJ31" s="28"/>
-      <c r="BK31" s="34" t="s">
+      <c r="BJ31" s="23"/>
+      <c r="BK31" s="28" t="s">
         <v>290</v>
       </c>
       <c r="BL31" s="4">
         <v>26</v>
       </c>
-      <c r="BM31" s="23" t="s">
+      <c r="BM31" s="18" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="9" t="s">
         <v>291</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -6078,19 +6118,19 @@
       <c r="BI32" s="2">
         <v>2</v>
       </c>
-      <c r="BJ32" s="29"/>
-      <c r="BK32" s="35" t="s">
+      <c r="BJ32" s="24"/>
+      <c r="BK32" s="29" t="s">
         <v>295</v>
       </c>
       <c r="BL32" s="2">
         <v>25</v>
       </c>
-      <c r="BM32" s="24" t="s">
+      <c r="BM32" s="19" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="33" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="10" t="s">
         <v>296</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -6234,220 +6274,215 @@
       <c r="BI33" s="4">
         <v>2</v>
       </c>
-      <c r="BJ33" s="28" t="s">
+      <c r="BJ33" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="BK33" s="34" t="s">
+      <c r="BK33" s="28" t="s">
         <v>304</v>
       </c>
       <c r="BL33" s="4">
         <v>28</v>
       </c>
-      <c r="BM33" s="23" t="s">
+      <c r="BM33" s="18" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="34" spans="2:65" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="D34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="22" t="s">
+      <c r="D34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="G34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="22" t="s">
+      <c r="G34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="J34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="K34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="L34" s="22" t="s">
+      <c r="J34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="M34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="N34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="O34" s="22" t="s">
+      <c r="M34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="O34" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="P34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="R34" s="22" t="s">
+      <c r="P34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="R34" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="S34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="T34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="U34" s="22" t="s">
+      <c r="S34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="T34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="U34" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="V34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="W34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="X34" s="22" t="s">
+      <c r="V34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="W34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="X34" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="Y34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA34" s="22" t="s">
+      <c r="Y34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA34" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="AB34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD34" s="22" t="s">
+      <c r="AB34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD34" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="AE34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG34" s="22" t="s">
+      <c r="AE34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG34" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="AH34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM34" s="22" t="s">
+      <c r="AH34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM34" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="AN34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AP34" s="22" t="s">
+      <c r="AN34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP34" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="AQ34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AR34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AS34" s="22" t="s">
+      <c r="AQ34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS34" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="AT34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AV34" s="22" t="s">
+      <c r="AT34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AU34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV34" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="AW34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AX34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AY34" s="22" t="s">
+      <c r="AW34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AX34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY34" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="AZ34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BA34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BB34" s="22" t="s">
+      <c r="AZ34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BA34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB34" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="BC34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BD34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BE34" s="22" t="s">
+      <c r="BC34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BD34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BE34" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="BF34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BG34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BH34" s="22" t="s">
+      <c r="BF34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH34" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="BI34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BJ34" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="BK34" s="36" t="s">
+      <c r="BI34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BJ34" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="BK34" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="BL34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="BM34" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>325</v>
+      <c r="BL34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BM34" s="20" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="BE4:BG4"/>
     <mergeCell ref="BH4:BJ4"/>
     <mergeCell ref="BK4:BM4"/>
@@ -6457,19 +6492,23 @@
     <mergeCell ref="AV4:AX4"/>
     <mergeCell ref="AY4:BA4"/>
     <mergeCell ref="BB4:BD4"/>
+    <mergeCell ref="AJ4:AL4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
     <mergeCell ref="U4:W4"/>
     <mergeCell ref="X4:Z4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="AG4:AI4"/>
-    <mergeCell ref="AJ4:AL4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
   </mergeCells>
+  <conditionalFormatting sqref="B5:C5 C4">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Nom"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Récupérations et affichages  des données dans le template
</commit_message>
<xml_diff>
--- a/backend/uploads/Feuil2.xlsx
+++ b/backend/uploads/Feuil2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD17043-C758-403F-8E1F-95F1AA75FCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC0AA94-3124-48B4-AE97-6FE1267029A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{283D1B77-55FE-45D0-8D91-BD52EDA226B8}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{283D1B77-55FE-45D0-8D91-BD52EDA226B8}"/>
   </bookViews>
   <sheets>
     <sheet name="L-M1 MAPI ALT 1 - ALT Semes-1" sheetId="1" r:id="rId1"/>
@@ -1399,27 +1399,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1743,7 +1733,7 @@
   <dimension ref="B1:BM34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1826,109 +1816,109 @@
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="34" t="s">
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="34" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="34" t="s">
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="34" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="34" t="s">
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="34" t="s">
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="34" t="s">
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="34" t="s">
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="34" t="s">
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="AH4" s="35"/>
-      <c r="AI4" s="35"/>
-      <c r="AJ4" s="34" t="s">
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="AK4" s="35"/>
-      <c r="AL4" s="35"/>
-      <c r="AM4" s="34" t="s">
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="AN4" s="35"/>
-      <c r="AO4" s="35"/>
-      <c r="AP4" s="34" t="s">
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="36"/>
+      <c r="AP4" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="AQ4" s="35"/>
-      <c r="AR4" s="35"/>
-      <c r="AS4" s="34" t="s">
+      <c r="AQ4" s="36"/>
+      <c r="AR4" s="36"/>
+      <c r="AS4" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="AT4" s="35"/>
-      <c r="AU4" s="35"/>
-      <c r="AV4" s="34" t="s">
+      <c r="AT4" s="36"/>
+      <c r="AU4" s="36"/>
+      <c r="AV4" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="AW4" s="35"/>
-      <c r="AX4" s="35"/>
-      <c r="AY4" s="34" t="s">
+      <c r="AW4" s="36"/>
+      <c r="AX4" s="36"/>
+      <c r="AY4" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="AZ4" s="35"/>
-      <c r="BA4" s="35"/>
-      <c r="BB4" s="34" t="s">
+      <c r="AZ4" s="36"/>
+      <c r="BA4" s="36"/>
+      <c r="BB4" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="BC4" s="35"/>
-      <c r="BD4" s="35"/>
-      <c r="BE4" s="34" t="s">
+      <c r="BC4" s="36"/>
+      <c r="BD4" s="36"/>
+      <c r="BE4" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="BF4" s="35"/>
-      <c r="BG4" s="35"/>
-      <c r="BH4" s="34" t="s">
+      <c r="BF4" s="36"/>
+      <c r="BG4" s="36"/>
+      <c r="BH4" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="BI4" s="35"/>
-      <c r="BJ4" s="35"/>
-      <c r="BK4" s="36" t="s">
+      <c r="BI4" s="36"/>
+      <c r="BJ4" s="36"/>
+      <c r="BK4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="BL4" s="37"/>
-      <c r="BM4" s="38"/>
+      <c r="BL4" s="38"/>
+      <c r="BM4" s="39"/>
     </row>
     <row r="5" spans="2:65" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="34" t="s">
         <v>325</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -6504,7 +6494,7 @@
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="AG4:AI4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:C5 C4">
+  <conditionalFormatting sqref="C4 B5:C5">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Nom"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mise en place du calcul des moyennes pondérées
</commit_message>
<xml_diff>
--- a/backend/uploads/Feuil2.xlsx
+++ b/backend/uploads/Feuil2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC0AA94-3124-48B4-AE97-6FE1267029A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B18A87E-D302-4F4A-9BF7-DDE15DDC895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{283D1B77-55FE-45D0-8D91-BD52EDA226B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{283D1B77-55FE-45D0-8D91-BD52EDA226B8}"/>
   </bookViews>
   <sheets>
     <sheet name="L-M1 MAPI ALT 1 - ALT Semes-1" sheetId="1" r:id="rId1"/>
@@ -1733,7 +1733,7 @@
   <dimension ref="B1:BM34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="BK6" sqref="BK6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6473,15 +6473,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="BE4:BG4"/>
-    <mergeCell ref="BH4:BJ4"/>
-    <mergeCell ref="BK4:BM4"/>
-    <mergeCell ref="AM4:AO4"/>
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AS4:AU4"/>
-    <mergeCell ref="AV4:AX4"/>
-    <mergeCell ref="AY4:BA4"/>
-    <mergeCell ref="BB4:BD4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:K4"/>
@@ -6493,6 +6484,15 @@
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="AG4:AI4"/>
+    <mergeCell ref="BE4:BG4"/>
+    <mergeCell ref="BH4:BJ4"/>
+    <mergeCell ref="BK4:BM4"/>
+    <mergeCell ref="AM4:AO4"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AS4:AU4"/>
+    <mergeCell ref="AV4:AX4"/>
+    <mergeCell ref="AY4:BA4"/>
+    <mergeCell ref="BB4:BD4"/>
   </mergeCells>
   <conditionalFormatting sqref="C4 B5:C5">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">

</xml_diff>